<commit_message>
commit formatacao condicional e etc
</commit_message>
<xml_diff>
--- a/Investimentos.xlsx
+++ b/Investimentos.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,25 +42,42 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFC7CE"/>
+          <bgColor rgb="00FFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00C6F4CE"/>
+          <bgColor rgb="00C6F4CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -425,274 +439,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Valor</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>VPA</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Teto 9%</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Valor Justo por Ação</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Margem Líquida</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>LPA</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>DY</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>EY</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>EY2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>P/L</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>P/VP</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>ROE</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>ROIC</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Tag Along</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>EV/EBITDA</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Dívida Líquida/Patrimônio</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Dívida Líquida/Ebitida</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Liq. Corrente</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>petr4</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>34.68</v>
-      </c>
-      <c r="C2" t="n">
-        <v>31.25</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.5821037999999999</v>
-      </c>
-      <c r="E2" t="n">
-        <v>79.50530642667822</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>23,67%</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="H2" t="n">
-        <v>18.65</v>
-      </c>
-      <c r="I2" t="n">
-        <v>25.92272202998846</v>
-      </c>
-      <c r="J2" t="n">
-        <v>90.10957324106114</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>3,86</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1,11</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>28,77%</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>19,56%</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>100 %</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2,68</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0,56</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0,88</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>1,08</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>vale3</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>60.62</v>
-      </c>
-      <c r="C3" t="n">
-        <v>41.24</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.6290537399999999</v>
-      </c>
-      <c r="E3" t="n">
-        <v>88.96621268773893</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>18,78%</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>8.529999999999999</v>
-      </c>
-      <c r="H3" t="n">
-        <v>11.53</v>
-      </c>
-      <c r="I3" t="n">
-        <v>14.07126360936984</v>
-      </c>
-      <c r="J3" t="n">
-        <v>68.03035301880568</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>7,11</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>1,47</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>20,68%</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>18,00%</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>100 %</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>4,19</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0,29</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0,69</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>1,12</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula/>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="1">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="greaterThanOrEqual" dxfId="2">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
formatação condicional + correção de função
</commit_message>
<xml_diff>
--- a/Investimentos.xlsx
+++ b/Investimentos.xlsx
@@ -68,24 +68,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-          <bgColor rgb="00FFFFFF"/>
+          <fgColor rgb="0092D050"/>
+          <bgColor rgb="0092D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFC7CE"/>
-          <bgColor rgb="00FFC7CE"/>
+          <fgColor rgb="00FF0000"/>
+          <bgColor rgb="00FF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00C6F4CE"/>
-          <bgColor rgb="00C6F4CE"/>
+          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -560,75 +560,374 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mglu3</t>
+          <t>petr4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.82</v>
+        <v>38.62</v>
       </c>
       <c r="C2" t="n">
-        <v>14.75</v>
+        <v>31.25</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>72.09066666666666</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>79.50530642667822</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.52</v>
+        <v>23.67</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.76</v>
+        <v>8.99</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="I2" t="n">
-        <v>-6.429780033840947</v>
+        <v>23.27809425168307</v>
       </c>
       <c r="J2" t="n">
-        <v>124.7884940778342</v>
+        <v>80.91662351113413</v>
       </c>
       <c r="K2" t="n">
-        <v>-15.6</v>
+        <v>4.3</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8</v>
+        <v>1.24</v>
       </c>
       <c r="M2" t="n">
-        <v>-5.14</v>
+        <v>28.77</v>
       </c>
       <c r="N2" t="n">
-        <v>-5.33</v>
+        <v>19.56</v>
       </c>
       <c r="O2" t="n">
         <v>100</v>
       </c>
       <c r="P2" t="n">
-        <v>10.62</v>
+        <v>2.89</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="R2" t="n">
-        <v>3.52</v>
+        <v>0.88</v>
       </c>
       <c r="S2" t="n">
-        <v>1.26</v>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>vale3</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>62.7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>41.24</v>
+      </c>
+      <c r="D3" t="n">
+        <v>76.91199999999999</v>
+      </c>
+      <c r="E3" t="n">
+        <v>88.96621268773893</v>
+      </c>
+      <c r="F3" t="n">
+        <v>18.78</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.529999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>11.04</v>
+      </c>
+      <c r="I3" t="n">
+        <v>13.60446570972887</v>
+      </c>
+      <c r="J3" t="n">
+        <v>65.77352472089314</v>
+      </c>
+      <c r="K3" t="n">
+        <v>7.42</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M3" t="n">
+        <v>20.68</v>
+      </c>
+      <c r="N3" t="n">
+        <v>18</v>
+      </c>
+      <c r="O3" t="n">
+        <v>100</v>
+      </c>
+      <c r="P3" t="n">
+        <v>4.35</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cmig3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12.41</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8.880000000000001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>14.87821111111111</v>
+      </c>
+      <c r="E4" t="n">
+        <v>19.63705680594727</v>
+      </c>
+      <c r="F4" t="n">
+        <v>14.81</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.79</v>
+      </c>
+      <c r="I4" t="n">
+        <v>15.55197421434327</v>
+      </c>
+      <c r="J4" t="n">
+        <v>71.55519742143433</v>
+      </c>
+      <c r="K4" t="n">
+        <v>6.53</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="M4" t="n">
+        <v>21.72</v>
+      </c>
+      <c r="N4" t="n">
+        <v>16.13</v>
+      </c>
+      <c r="O4" t="n">
+        <v>80</v>
+      </c>
+      <c r="P4" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>azul4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7.12</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-17.69</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>22.47191011235955</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-248.4550561797753</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-0.41</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-9.06</v>
+      </c>
+      <c r="N5" t="n">
+        <v>43.38</v>
+      </c>
+      <c r="O5" t="n">
+        <v>100</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.34</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
-      <formula/>
+  <conditionalFormatting sqref="F2:F5">
+    <cfRule type="cellIs" priority="1" operator="greaterThanOrEqual" dxfId="0">
+      <formula>10</formula>
     </cfRule>
     <cfRule type="cellIs" priority="2" operator="between" dxfId="1">
       <formula>0.001</formula>
       <formula>9.999</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="greaterThanOrEqual" dxfId="2">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q5">
+    <cfRule type="cellIs" priority="4" operator="between" dxfId="0">
+      <formula>0.001</formula>
+      <formula>0.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="greaterThanOrEqual" dxfId="1">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N5">
+    <cfRule type="cellIs" priority="7" operator="greaterThanOrEqual" dxfId="0">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="between" dxfId="1">
+      <formula>0.001</formula>
+      <formula>14.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R5">
+    <cfRule type="cellIs" priority="10" operator="between" dxfId="0">
+      <formula>0.001</formula>
+      <formula>2.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="greaterThanOrEqual" dxfId="1">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O5">
+    <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="14" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K5">
+    <cfRule type="cellIs" priority="15" operator="between" dxfId="0">
+      <formula>0.001</formula>
+      <formula>9.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="16" operator="greaterThanOrEqual" dxfId="1">
       <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="17" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L5">
+    <cfRule type="cellIs" priority="18" operator="between" dxfId="0">
+      <formula>0.001</formula>
+      <formula>1.499</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="19" operator="greaterThanOrEqual" dxfId="1">
+      <formula>1.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="20" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S5">
+    <cfRule type="cellIs" priority="21" operator="greaterThanOrEqual" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="22" operator="between" dxfId="1">
+      <formula>0.001</formula>
+      <formula>0.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="23" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M5">
+    <cfRule type="cellIs" priority="24" operator="greaterThanOrEqual" dxfId="0">
+      <formula>16</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="25" operator="between" dxfId="1">
+      <formula>0.001</formula>
+      <formula>15.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="26" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P5">
+    <cfRule type="cellIs" priority="27" operator="between" dxfId="0">
+      <formula>0.001</formula>
+      <formula>4.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="28" operator="greaterThanOrEqual" dxfId="1">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="29" operator="equal" dxfId="2">
+      <formula/>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I5">
+    <cfRule type="cellIs" priority="30" operator="greaterThanOrEqual" dxfId="0">
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="31" operator="between" dxfId="1">
+      <formula>0.001</formula>
+      <formula>19.999</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="32" operator="equal" dxfId="2">
+      <formula/>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
commit de pequenas modificações
</commit_message>
<xml_diff>
--- a/Investimentos.xlsx
+++ b/Investimentos.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -564,55 +564,55 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>38.62</v>
+        <v>37.34</v>
       </c>
       <c r="C2" t="n">
         <v>31.25</v>
       </c>
       <c r="D2" t="n">
-        <v>72.09066666666666</v>
+        <v>71.98322222222224</v>
       </c>
       <c r="E2" t="n">
-        <v>79.50530642667822</v>
+        <v>77.034894690653</v>
       </c>
       <c r="F2" t="n">
-        <v>23.67</v>
+        <v>22.45</v>
       </c>
       <c r="G2" t="n">
-        <v>8.99</v>
+        <v>8.44</v>
       </c>
       <c r="H2" t="n">
-        <v>16.8</v>
+        <v>17.35</v>
       </c>
       <c r="I2" t="n">
-        <v>23.27809425168307</v>
+        <v>22.60310658810926</v>
       </c>
       <c r="J2" t="n">
-        <v>80.91662351113413</v>
+        <v>83.69041242635244</v>
       </c>
       <c r="K2" t="n">
-        <v>4.3</v>
+        <v>4.43</v>
       </c>
       <c r="L2" t="n">
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
       <c r="M2" t="n">
-        <v>28.77</v>
+        <v>27.02</v>
       </c>
       <c r="N2" t="n">
-        <v>19.56</v>
+        <v>17.93</v>
       </c>
       <c r="O2" t="n">
         <v>100</v>
       </c>
       <c r="P2" t="n">
-        <v>2.89</v>
+        <v>3.07</v>
       </c>
       <c r="Q2" t="n">
         <v>0.5600000000000001</v>
       </c>
       <c r="R2" t="n">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>1.08</v>
@@ -621,188 +621,127 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>vale3</t>
+          <t>cmig3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>62.7</v>
+        <v>12.93</v>
       </c>
       <c r="C3" t="n">
-        <v>41.24</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>76.91199999999999</v>
+        <v>15.07063333333333</v>
       </c>
       <c r="E3" t="n">
-        <v>88.96621268773893</v>
+        <v>19.63705680594727</v>
       </c>
       <c r="F3" t="n">
-        <v>18.78</v>
+        <v>14.81</v>
       </c>
       <c r="G3" t="n">
-        <v>8.529999999999999</v>
+        <v>1.93</v>
       </c>
       <c r="H3" t="n">
-        <v>11.04</v>
+        <v>10.49</v>
       </c>
       <c r="I3" t="n">
-        <v>13.60446570972887</v>
+        <v>14.92652745552978</v>
       </c>
       <c r="J3" t="n">
-        <v>65.77352472089314</v>
+        <v>68.67749419953597</v>
       </c>
       <c r="K3" t="n">
-        <v>7.42</v>
+        <v>6.71</v>
       </c>
       <c r="L3" t="n">
-        <v>1.53</v>
+        <v>1.46</v>
       </c>
       <c r="M3" t="n">
-        <v>20.68</v>
+        <v>21.72</v>
       </c>
       <c r="N3" t="n">
-        <v>18</v>
+        <v>16.13</v>
       </c>
       <c r="O3" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P3" t="n">
-        <v>4.35</v>
+        <v>4.76</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.29</v>
+        <v>0.28</v>
       </c>
       <c r="R3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="S3" t="n">
-        <v>1.12</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cmig3</t>
+          <t>sbsp3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.41</v>
+        <v>88.65000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>8.880000000000001</v>
+        <v>44.89</v>
       </c>
       <c r="D4" t="n">
-        <v>14.87821111111111</v>
+        <v>16.0555</v>
       </c>
       <c r="E4" t="n">
-        <v>19.63705680594727</v>
+        <v>72.95773947978377</v>
       </c>
       <c r="F4" t="n">
-        <v>14.81</v>
+        <v>13.62</v>
       </c>
       <c r="G4" t="n">
-        <v>1.93</v>
+        <v>5.27</v>
       </c>
       <c r="H4" t="n">
-        <v>10.79</v>
+        <v>1.63</v>
       </c>
       <c r="I4" t="n">
-        <v>15.55197421434327</v>
+        <v>5.944726452340665</v>
       </c>
       <c r="J4" t="n">
-        <v>71.55519742143433</v>
+        <v>50.63733784545968</v>
       </c>
       <c r="K4" t="n">
-        <v>6.53</v>
+        <v>16.82</v>
       </c>
       <c r="L4" t="n">
-        <v>1.42</v>
+        <v>1.97</v>
       </c>
       <c r="M4" t="n">
-        <v>21.72</v>
+        <v>11.73</v>
       </c>
       <c r="N4" t="n">
-        <v>16.13</v>
+        <v>10</v>
       </c>
       <c r="O4" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="P4" t="n">
-        <v>4.63</v>
+        <v>7.94</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.28</v>
+        <v>0.52</v>
       </c>
       <c r="R4" t="n">
-        <v>0.86</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>1.15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>azul4</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>7.12</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-17.69</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>10.81</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>22.47191011235955</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-248.4550561797753</v>
-      </c>
-      <c r="K5" t="n">
-        <v>4.55</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-0.41</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-9.06</v>
-      </c>
-      <c r="N5" t="n">
-        <v>43.38</v>
-      </c>
-      <c r="O5" t="n">
-        <v>100</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.34</v>
+        <v>1.23</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F5">
+  <conditionalFormatting sqref="F2:F4">
     <cfRule type="cellIs" priority="1" operator="greaterThanOrEqual" dxfId="0">
       <formula>10</formula>
     </cfRule>
@@ -814,7 +753,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q5">
+  <conditionalFormatting sqref="Q2:Q4">
     <cfRule type="cellIs" priority="4" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>0.999</formula>
@@ -826,7 +765,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N5">
+  <conditionalFormatting sqref="N2:N4">
     <cfRule type="cellIs" priority="7" operator="greaterThanOrEqual" dxfId="0">
       <formula>15</formula>
     </cfRule>
@@ -838,7 +777,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R5">
+  <conditionalFormatting sqref="R2:R4">
     <cfRule type="cellIs" priority="10" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>2.999</formula>
@@ -850,7 +789,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O5">
+  <conditionalFormatting sqref="O2:O4">
     <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
       <formula>100</formula>
     </cfRule>
@@ -858,7 +797,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K5">
+  <conditionalFormatting sqref="K2:K4">
     <cfRule type="cellIs" priority="15" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>9.999</formula>
@@ -870,7 +809,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L5">
+  <conditionalFormatting sqref="L2:L4">
     <cfRule type="cellIs" priority="18" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>1.499</formula>
@@ -882,7 +821,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S5">
+  <conditionalFormatting sqref="S2:S4">
     <cfRule type="cellIs" priority="21" operator="greaterThanOrEqual" dxfId="0">
       <formula>1</formula>
     </cfRule>
@@ -894,7 +833,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M5">
+  <conditionalFormatting sqref="M2:M4">
     <cfRule type="cellIs" priority="24" operator="greaterThanOrEqual" dxfId="0">
       <formula>16</formula>
     </cfRule>
@@ -906,7 +845,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P5">
+  <conditionalFormatting sqref="P2:P4">
     <cfRule type="cellIs" priority="27" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>4.999</formula>
@@ -918,7 +857,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="30" operator="greaterThanOrEqual" dxfId="0">
       <formula>20</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mudanças para melhor experiência do usuário
</commit_message>
<xml_diff>
--- a/Investimentos.xlsx
+++ b/Investimentos.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.51</v>
+        <v>38.5</v>
       </c>
       <c r="C2" t="n">
         <v>31.25</v>
@@ -586,16 +586,16 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>16.54341276362641</v>
+        <v>15.68831168831169</v>
       </c>
       <c r="J2" t="n">
-        <v>85.59298822240481</v>
+        <v>81.16883116883116</v>
       </c>
       <c r="K2" t="n">
-        <v>6.05</v>
+        <v>6.38</v>
       </c>
       <c r="L2" t="n">
-        <v>1.17</v>
+        <v>1.23</v>
       </c>
       <c r="M2" t="n">
         <v>19.32</v>
@@ -607,7 +607,7 @@
         <v>100</v>
       </c>
       <c r="P2" t="n">
-        <v>3.11</v>
+        <v>3.23</v>
       </c>
       <c r="Q2" t="n">
         <v>0.5600000000000001</v>
@@ -619,132 +619,8 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>vale3</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>57.06</v>
-      </c>
-      <c r="C3" t="n">
-        <v>45.26</v>
-      </c>
-      <c r="D3">
-        <f>(H3*B3)/9</f>
-        <v/>
-      </c>
-      <c r="E3" t="n">
-        <v>104.5804905324124</v>
-      </c>
-      <c r="F3" t="n">
-        <v>23.19</v>
-      </c>
-      <c r="G3" t="n">
-        <v>10.74</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>18.82229232386961</v>
-      </c>
-      <c r="J3" t="n">
-        <v>79.32001402032947</v>
-      </c>
-      <c r="K3" t="n">
-        <v>5.32</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.26</v>
-      </c>
-      <c r="M3" t="n">
-        <v>23.72</v>
-      </c>
-      <c r="N3" t="n">
-        <v>21.52</v>
-      </c>
-      <c r="O3" t="n">
-        <v>100</v>
-      </c>
-      <c r="P3" t="n">
-        <v>3.65</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>beef3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>7.51</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="D4">
-        <f>(H4*B4)/9</f>
-        <v/>
-      </c>
-      <c r="E4" t="n">
-        <v>1.723368793961409</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.597869507323569</v>
-      </c>
-      <c r="J4" t="n">
-        <v>14.64713715046605</v>
-      </c>
-      <c r="K4" t="n">
-        <v>64.45</v>
-      </c>
-      <c r="L4" t="n">
-        <v>6.81</v>
-      </c>
-      <c r="M4" t="n">
-        <v>10.57</v>
-      </c>
-      <c r="N4" t="n">
-        <v>7.73</v>
-      </c>
-      <c r="O4" t="n">
-        <v>100</v>
-      </c>
-      <c r="P4" t="n">
-        <v>5.25</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>14.3</v>
-      </c>
-      <c r="R4" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="S4" t="n">
-        <v>2.22</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F4">
+  <conditionalFormatting sqref="F2">
     <cfRule type="cellIs" priority="1" operator="greaterThanOrEqual" dxfId="0">
       <formula>10</formula>
     </cfRule>
@@ -756,7 +632,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q4">
+  <conditionalFormatting sqref="Q2">
     <cfRule type="cellIs" priority="4" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>0.999</formula>
@@ -768,7 +644,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N4">
+  <conditionalFormatting sqref="N2">
     <cfRule type="cellIs" priority="7" operator="greaterThanOrEqual" dxfId="0">
       <formula>15</formula>
     </cfRule>
@@ -780,7 +656,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R4">
+  <conditionalFormatting sqref="R2">
     <cfRule type="cellIs" priority="10" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>2.999</formula>
@@ -792,7 +668,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O4">
+  <conditionalFormatting sqref="O2">
     <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
       <formula>100</formula>
     </cfRule>
@@ -800,7 +676,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K4">
+  <conditionalFormatting sqref="K2">
     <cfRule type="cellIs" priority="15" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>9.999</formula>
@@ -812,7 +688,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L4">
+  <conditionalFormatting sqref="L2">
     <cfRule type="cellIs" priority="18" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>1.499</formula>
@@ -824,7 +700,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S4">
+  <conditionalFormatting sqref="S2">
     <cfRule type="cellIs" priority="21" operator="greaterThanOrEqual" dxfId="0">
       <formula>1</formula>
     </cfRule>
@@ -836,7 +712,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M4">
+  <conditionalFormatting sqref="M2">
     <cfRule type="cellIs" priority="24" operator="greaterThanOrEqual" dxfId="0">
       <formula>16</formula>
     </cfRule>
@@ -848,7 +724,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P4">
+  <conditionalFormatting sqref="P2">
     <cfRule type="cellIs" priority="27" operator="between" dxfId="0">
       <formula>0.001</formula>
       <formula>4.999</formula>
@@ -860,7 +736,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" priority="30" operator="greaterThanOrEqual" dxfId="0">
       <formula>20</formula>
     </cfRule>
@@ -872,7 +748,7 @@
       <formula/>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" priority="33" operator="greaterThanOrEqual" dxfId="0">
       <formula>25</formula>
     </cfRule>
@@ -886,11 +762,11 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" priority="36" operator="greaterThanOrEqual" dxfId="0">
-      <formula>36.51</formula>
+      <formula>38.5</formula>
     </cfRule>
     <cfRule type="cellIs" priority="37" operator="between" dxfId="1">
       <formula>0.001</formula>
-      <formula>36.509</formula>
+      <formula>38.499</formula>
     </cfRule>
     <cfRule type="cellIs" priority="38" operator="equal" dxfId="2">
       <formula/>
@@ -898,11 +774,11 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
     <cfRule type="cellIs" priority="39" operator="greaterThanOrEqual" dxfId="0">
-      <formula>36.51</formula>
+      <formula>38.5</formula>
     </cfRule>
     <cfRule type="cellIs" priority="40" operator="between" dxfId="1">
       <formula>0.001</formula>
-      <formula>36.509</formula>
+      <formula>38.499</formula>
     </cfRule>
     <cfRule type="cellIs" priority="41" operator="equal" dxfId="2">
       <formula/>
@@ -910,85 +786,13 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="cellIs" priority="42" operator="greaterThanOrEqual" dxfId="0">
-      <formula>36.51</formula>
+      <formula>38.5</formula>
     </cfRule>
     <cfRule type="cellIs" priority="43" operator="between" dxfId="1">
       <formula>0.001</formula>
-      <formula>36.509</formula>
+      <formula>38.499</formula>
     </cfRule>
     <cfRule type="cellIs" priority="44" operator="equal" dxfId="2">
-      <formula/>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" priority="45" operator="greaterThanOrEqual" dxfId="0">
-      <formula>57.06</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="46" operator="between" dxfId="1">
-      <formula>0.001</formula>
-      <formula>57.059000000000005</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="47" operator="equal" dxfId="2">
-      <formula/>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" priority="48" operator="greaterThanOrEqual" dxfId="0">
-      <formula>57.06</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="49" operator="between" dxfId="1">
-      <formula>0.001</formula>
-      <formula>57.059000000000005</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="50" operator="equal" dxfId="2">
-      <formula/>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" priority="51" operator="greaterThanOrEqual" dxfId="0">
-      <formula>57.06</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="52" operator="between" dxfId="1">
-      <formula>0.001</formula>
-      <formula>57.059000000000005</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="53" operator="equal" dxfId="2">
-      <formula/>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" priority="54" operator="greaterThanOrEqual" dxfId="0">
-      <formula>7.51</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="55" operator="between" dxfId="1">
-      <formula>0.001</formula>
-      <formula>7.5089999999999995</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="56" operator="equal" dxfId="2">
-      <formula/>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" priority="57" operator="greaterThanOrEqual" dxfId="0">
-      <formula>7.51</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="58" operator="between" dxfId="1">
-      <formula>0.001</formula>
-      <formula>7.5089999999999995</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="59" operator="equal" dxfId="2">
-      <formula/>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" priority="60" operator="greaterThanOrEqual" dxfId="0">
-      <formula>7.51</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="61" operator="between" dxfId="1">
-      <formula>0.001</formula>
-      <formula>7.5089999999999995</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="62" operator="equal" dxfId="2">
       <formula/>
     </cfRule>
   </conditionalFormatting>

</xml_diff>